<commit_message>
Added Test script for Customer Reg
</commit_message>
<xml_diff>
--- a/Passbrains Smoke Test Pack/src/grid/Suite1.xlsx
+++ b/Passbrains Smoke Test Pack/src/grid/Suite1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11115" windowHeight="4035"/>
+    <workbookView xWindow="675" yWindow="3390" windowWidth="19140" windowHeight="6270" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -12,15 +12,15 @@
     <sheet name="NoviceTester2Steps" sheetId="3" r:id="rId3"/>
     <sheet name="ProfessionalTester" sheetId="4" r:id="rId4"/>
     <sheet name="ProfTester3Steps" sheetId="5" r:id="rId5"/>
-    <sheet name="Customer" sheetId="6" r:id="rId6"/>
+    <sheet name="Customer" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:D12"/>
+  <oleSize ref="A1:L11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
   <si>
     <t>TCID</t>
   </si>
@@ -170,6 +170,33 @@
   </si>
   <si>
     <t>Android 4.3</t>
+  </si>
+  <si>
+    <t>Job_Title</t>
+  </si>
+  <si>
+    <t>Dept</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>passbrains</t>
+  </si>
+  <si>
+    <t>PassIndia</t>
+  </si>
+  <si>
+    <t>Information Technology and Services</t>
+  </si>
+  <si>
+    <t>9886863190</t>
   </si>
 </sst>
 </file>
@@ -564,7 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -650,7 +677,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,12 +966,94 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="6">
+        <v>363310</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Customer Registration - Working Code
</commit_message>
<xml_diff>
--- a/Passbrains Smoke Test Pack/src/grid/Suite1.xlsx
+++ b/Passbrains Smoke Test Pack/src/grid/Suite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="3390" windowWidth="19140" windowHeight="6270" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14115" windowHeight="6270" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,12 @@
     <sheet name="Customer" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L11"/>
+  <oleSize ref="A1:E19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
   <si>
     <t>TCID</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>9886863190</t>
+  </si>
+  <si>
+    <t>Phone_C</t>
   </si>
 </sst>
 </file>
@@ -592,7 +595,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,7 +667,7 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -676,7 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -968,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,7 +1012,7 @@
         <v>53</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Code Clean Up,assertions added
</commit_message>
<xml_diff>
--- a/Passbrains Smoke Test Pack/src/grid/Suite1.xlsx
+++ b/Passbrains Smoke Test Pack/src/grid/Suite1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="13605" windowHeight="3900" firstSheet="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11400" windowHeight="1950" firstSheet="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +674,7 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Close browser function to ALL
</commit_message>
<xml_diff>
--- a/Passbrains Smoke Test Pack/src/grid/Suite1.xlsx
+++ b/Passbrains Smoke Test Pack/src/grid/Suite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11400" windowHeight="1950" firstSheet="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11400" windowHeight="1950" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
     <sheet name="Customer_Tester" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G11"/>
+  <oleSize ref="F1:N5"/>
 </workbook>
 </file>
 
@@ -164,9 +164,6 @@
     <t>Samsung</t>
   </si>
   <si>
-    <t>Galaxy Nexus</t>
-  </si>
-  <si>
     <t>Vodafone India</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>Customer+Tester</t>
+  </si>
+  <si>
+    <t>Galaxy</t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -679,10 +679,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
         <v>60</v>
-      </c>
-      <c r="B7" t="s">
-        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,13 +941,13 @@
         <v>46</v>
       </c>
       <c r="Q2" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" t="s">
         <v>47</v>
-      </c>
-      <c r="R2" t="s">
-        <v>49</v>
-      </c>
-      <c r="S2" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1018,19 +1018,19 @@
         <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
@@ -1056,19 +1056,19 @@
         <v>34</v>
       </c>
       <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" t="s">
         <v>55</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>56</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1112,19 +1112,19 @@
         <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>26</v>
@@ -1156,19 +1156,19 @@
         <v>34</v>
       </c>
       <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" t="s">
         <v>55</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>56</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="M2">
         <v>1990</v>

</xml_diff>

<commit_message>
Modified Novice Tester 2 steps
</commit_message>
<xml_diff>
--- a/Passbrains Smoke Test Pack/src/grid/Suite1.xlsx
+++ b/Passbrains Smoke Test Pack/src/grid/Suite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11400" windowHeight="1950" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11400" windowHeight="3915" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="63">
   <si>
     <t>TCID</t>
   </si>
@@ -161,15 +161,9 @@
     <t>English</t>
   </si>
   <si>
-    <t>Samsung</t>
-  </si>
-  <si>
     <t>Vodafone India</t>
   </si>
   <si>
-    <t>Android 4.3</t>
-  </si>
-  <si>
     <t>Job_Title</t>
   </si>
   <si>
@@ -206,7 +200,16 @@
     <t>Customer+Tester</t>
   </si>
   <si>
-    <t>Galaxy</t>
+    <t>363310</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -679,10 +682,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -808,7 +811,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,8 +919,8 @@
       <c r="H2" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="6">
-        <v>363310</v>
+      <c r="I2" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="J2" t="s">
         <v>34</v>
@@ -937,17 +940,17 @@
       <c r="O2" t="s">
         <v>45</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" t="s">
+        <v>62</v>
+      </c>
+      <c r="S2" t="s">
         <v>46</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>61</v>
-      </c>
-      <c r="R2" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -956,6 +959,7 @@
     <hyperlink ref="F2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1018,19 +1022,19 @@
         <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
@@ -1056,19 +1060,19 @@
         <v>34</v>
       </c>
       <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" t="s">
         <v>54</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="K2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1112,19 +1116,19 @@
         <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>26</v>
@@ -1156,19 +1160,19 @@
         <v>34</v>
       </c>
       <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" t="s">
         <v>54</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="K2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="M2">
         <v>1990</v>

</xml_diff>

<commit_message>
Professional Testers registers with single Step and 3 Steps
</commit_message>
<xml_diff>
--- a/Passbrains Smoke Test Pack/src/grid/Suite1.xlsx
+++ b/Passbrains Smoke Test Pack/src/grid/Suite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11400" windowHeight="3915" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11400" windowHeight="3915" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,12 @@
     <sheet name="Customer_Tester" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:D11"/>
+  <oleSize ref="H1:R11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="64">
   <si>
     <t>TCID</t>
   </si>
@@ -41,9 +41,6 @@
     <t>City</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>NoviceTester</t>
   </si>
   <si>
@@ -210,6 +207,12 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -288,7 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -300,6 +303,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -604,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,10 +631,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -638,10 +642,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -649,32 +653,32 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -682,10 +686,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
         <v>57</v>
-      </c>
-      <c r="B7" t="s">
-        <v>58</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -700,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,80 +724,80 @@
     <col min="12" max="12" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>32</v>
-      </c>
-      <c r="H2" t="s">
-        <v>33</v>
       </c>
       <c r="I2" s="6">
         <v>363310</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K2">
         <v>1990</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -810,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,120 +841,120 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>32</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" t="s">
         <v>33</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
       </c>
       <c r="K2">
         <v>1990</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N2">
         <v>8</v>
       </c>
       <c r="O2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S2" t="s">
         <v>45</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R2" t="s">
-        <v>62</v>
-      </c>
-      <c r="S2" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -965,27 +969,261 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="6">
+        <v>363310</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2">
+        <v>1990</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="6">
+        <v>363310</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1988</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="3">
+        <v>8</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1001,78 +1239,78 @@
   <sheetData>
     <row r="1" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
         <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
       </c>
       <c r="F2" s="6">
         <v>363310</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" t="s">
         <v>52</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>53</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1095,90 +1333,90 @@
   <sheetData>
     <row r="1" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
         <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
       </c>
       <c r="F2" s="6">
         <v>363310</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" t="s">
         <v>52</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>53</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="M2">
         <v>1990</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mail Sending Capability Added
</commit_message>
<xml_diff>
--- a/Passbrains Smoke Test Pack/src/grid/Suite1.xlsx
+++ b/Passbrains Smoke Test Pack/src/grid/Suite1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14805" windowHeight="3660"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11400" windowHeight="2700" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Customer_Tester2steps" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H10"/>
+  <oleSize ref="A1:K7"/>
 </workbook>
 </file>
 
@@ -631,7 +631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1131,7 +1131,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,7 +1480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>